<commit_message>
1. Update Data. 2. Add new graphs. 3. Add new metadata.
</commit_message>
<xml_diff>
--- a/DashboardSW/data-in/Data-In.xlsx
+++ b/DashboardSW/data-in/Data-In.xlsx
@@ -244,9 +244,6 @@
     <t>xprlan101</t>
   </si>
   <si>
-    <t>74:46:A0:98:27:E4</t>
-  </si>
-  <si>
     <t>19-AUG-14 08.21.00.000000 PM</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>xprbee007</t>
   </si>
   <si>
-    <t>00:1F:29:41:37:E3</t>
-  </si>
-  <si>
     <t>18-AUG-14 05.45.00.000000 AM</t>
   </si>
   <si>
@@ -319,9 +313,6 @@
     <t>xprdpk070l</t>
   </si>
   <si>
-    <t>18:A9:05:90:14:20</t>
-  </si>
-  <si>
     <t>26-SEP-12 02.51.00.000000 PM</t>
   </si>
   <si>
@@ -355,9 +346,6 @@
     <t>xprdpk185</t>
   </si>
   <si>
-    <t>80:C1:6E:E1:7A:D9</t>
-  </si>
-  <si>
     <t>28-JUL-14 06.57.00.000000 AM</t>
   </si>
   <si>
@@ -385,9 +373,6 @@
     <t>xts331</t>
   </si>
   <si>
-    <t>00:21:5A:23:6F:88</t>
-  </si>
-  <si>
     <t>05-AUG-14 08.39.00.000000 AM</t>
   </si>
   <si>
@@ -418,9 +403,6 @@
     <t>xreglod080</t>
   </si>
   <si>
-    <t>00:25:B3:29:41:BD</t>
-  </si>
-  <si>
     <t>08-AUG-13 02.47.00.000000 PM</t>
   </si>
   <si>
@@ -448,9 +430,6 @@
     <t>xkits023</t>
   </si>
   <si>
-    <t>00:25:B3:CE:DB:1A</t>
-  </si>
-  <si>
     <t>22-MAY-14 12.53.00.000000 AM</t>
   </si>
   <si>
@@ -478,9 +457,6 @@
     <t>xccsun043</t>
   </si>
   <si>
-    <t>18:A9:05:B4:FF:19</t>
-  </si>
-  <si>
     <t>30-MAY-14 03.03.00.000000 PM</t>
   </si>
   <si>
@@ -508,9 +484,6 @@
     <t>xts293</t>
   </si>
   <si>
-    <t>00:21:5A:23:6F:94</t>
-  </si>
-  <si>
     <t>19-FEB-14 05.38.00.000000 AM</t>
   </si>
   <si>
@@ -535,9 +508,6 @@
     <t>xprbar139</t>
   </si>
   <si>
-    <t>18:A9:05:B6:B0:4D</t>
-  </si>
-  <si>
     <t>13-MAY-14 03.10.00.000000 PM</t>
   </si>
   <si>
@@ -623,6 +593,36 @@
   </si>
   <si>
     <t>HANDERSEN</t>
+  </si>
+  <si>
+    <t>47:64:0A:89:72:4E</t>
+  </si>
+  <si>
+    <t>99:F1:92:14:73:3E</t>
+  </si>
+  <si>
+    <t>81:9A:50:09:41:02</t>
+  </si>
+  <si>
+    <t>08:1C:E6:1E:A7:9D</t>
+  </si>
+  <si>
+    <t>00:12:A5:32:F6:58</t>
+  </si>
+  <si>
+    <t>73:52:3B:92:14:DB</t>
+  </si>
+  <si>
+    <t>58:52:3B:E4:B8:A2</t>
+  </si>
+  <si>
+    <t>81:9A:5F:4B:BF:91</t>
+  </si>
+  <si>
+    <t>92:12:A4:37:F3:45</t>
+  </si>
+  <si>
+    <t>89:9C:5D:65:07:D6</t>
   </si>
 </sst>
 </file>
@@ -967,9 +967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="AQ10" sqref="AQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
         <v>41471</v>
       </c>
       <c r="H2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
         <v>46</v>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="U2">
         <v>16351</v>
@@ -1217,16 +1217,16 @@
         <v>53</v>
       </c>
       <c r="X2" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y2" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" t="s">
-        <v>167</v>
-      </c>
       <c r="Z2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA2" t="s">
         <v>54</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>55</v>
       </c>
       <c r="AB2">
         <v>6851</v>
@@ -1238,10 +1238,10 @@
         <v>11151</v>
       </c>
       <c r="AE2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" t="s">
         <v>56</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>57</v>
       </c>
       <c r="AG2" s="1">
         <v>41696.74858796296</v>
@@ -1256,16 +1256,16 @@
         <v>0</v>
       </c>
       <c r="AK2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" t="s">
-        <v>59</v>
-      </c>
       <c r="AM2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="AN2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="AP2" s="1">
         <v>41879.430219907408</v>
@@ -1282,19 +1282,19 @@
         <v>42</v>
       </c>
       <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
       </c>
       <c r="G3" s="1">
         <v>39281</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I3" t="s">
         <v>46</v>
@@ -1303,16 +1303,16 @@
         <v>46</v>
       </c>
       <c r="K3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="s">
         <v>63</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
       </c>
       <c r="M3" t="s">
         <v>49</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O3">
         <v>2050280</v>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="U3">
         <v>5050</v>
@@ -1339,19 +1339,19 @@
         <v>1</v>
       </c>
       <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA3" t="s">
         <v>66</v>
-      </c>
-      <c r="X3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>68</v>
       </c>
       <c r="AB3">
         <v>2926</v>
@@ -1363,10 +1363,10 @@
         <v>13734</v>
       </c>
       <c r="AE3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AF3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG3" s="1">
         <v>40808.651956018519</v>
@@ -1381,16 +1381,16 @@
         <v>0</v>
       </c>
       <c r="AK3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AL3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AM3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="AN3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="AP3" s="1">
         <v>41879.420752314814</v>
@@ -1407,19 +1407,19 @@
         <v>42</v>
       </c>
       <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
         <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="1">
         <v>39891</v>
       </c>
       <c r="H4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="I4" t="s">
         <v>46</v>
@@ -1428,16 +1428,16 @@
         <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M4" t="s">
         <v>49</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O4">
         <v>2023628</v>
@@ -1455,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="U4">
         <v>14387</v>
@@ -1464,19 +1464,19 @@
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="X4" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="Y4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="Z4" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="AA4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AB4">
         <v>1421</v>
@@ -1488,10 +1488,10 @@
         <v>735366</v>
       </c>
       <c r="AE4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AF4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG4" s="1">
         <v>41495.977534722224</v>
@@ -1506,16 +1506,16 @@
         <v>3</v>
       </c>
       <c r="AK4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AL4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="AN4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="AP4" s="1">
         <v>41794.65960648148</v>
@@ -1532,19 +1532,19 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G5" s="1">
         <v>40857</v>
       </c>
       <c r="H5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
@@ -1553,16 +1553,16 @@
         <v>46</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
       </c>
       <c r="N5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O5">
         <v>3319760</v>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="U5">
         <v>12800</v>
@@ -1589,19 +1589,19 @@
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="Y5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="Z5" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="AA5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AB5">
         <v>11712</v>
@@ -1613,10 +1613,10 @@
         <v>43512</v>
       </c>
       <c r="AE5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AF5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG5" s="1">
         <v>41321.018425925926</v>
@@ -1631,16 +1631,16 @@
         <v>0</v>
       </c>
       <c r="AK5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AL5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AM5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="AN5" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="AP5" s="1">
         <v>41879.424884259257</v>
@@ -1657,19 +1657,19 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G6" s="1">
         <v>39281</v>
       </c>
       <c r="H6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
         <v>46</v>
@@ -1678,16 +1678,16 @@
         <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M6" t="s">
         <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O6">
         <v>2050280</v>
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U6">
         <v>10694</v>
@@ -1714,19 +1714,19 @@
         <v>1</v>
       </c>
       <c r="W6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="X6" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="Y6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z6" t="s">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="AA6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="AB6">
         <v>8315</v>
@@ -1738,10 +1738,10 @@
         <v>31881</v>
       </c>
       <c r="AE6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="AF6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG6" s="1">
         <v>41096.963252314818</v>
@@ -1756,16 +1756,16 @@
         <v>0</v>
       </c>
       <c r="AK6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AL6" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="AM6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="AN6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="AP6" s="1">
         <v>41879.463703703703</v>
@@ -1782,13 +1782,13 @@
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G7" s="1">
         <v>39936</v>
@@ -1797,16 +1797,16 @@
         <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M7" t="s">
         <v>49</v>
       </c>
       <c r="N7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O7">
         <v>2024624</v>
@@ -1824,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="T7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U7">
         <v>14370</v>
@@ -1833,19 +1833,19 @@
         <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="X7" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Y7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z7" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="AA7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AB7">
         <v>0</v>
@@ -1857,10 +1857,10 @@
         <v>12</v>
       </c>
       <c r="AE7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AF7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG7" s="1">
         <v>41594.016585648147</v>
@@ -1875,16 +1875,16 @@
         <v>3</v>
       </c>
       <c r="AK7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="AL7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="AM7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AN7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="AP7" s="1">
         <v>41771.603217592594</v>
@@ -1901,19 +1901,19 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G8" s="1">
         <v>39877</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="I8" t="s">
         <v>46</v>
@@ -1922,16 +1922,16 @@
         <v>46</v>
       </c>
       <c r="K8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="L8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M8" t="s">
         <v>49</v>
       </c>
       <c r="N8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O8">
         <v>2024624</v>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="T8" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U8">
         <v>8400</v>
@@ -1958,19 +1958,19 @@
         <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="X8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Y8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z8" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="AA8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="AB8">
         <v>22960</v>
@@ -1982,10 +1982,10 @@
         <v>140266</v>
       </c>
       <c r="AE8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="AF8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG8" s="1">
         <v>40824.003460648149</v>
@@ -2000,19 +2000,19 @@
         <v>0</v>
       </c>
       <c r="AK8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="AL8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="AM8" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="AN8" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="AO8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="AP8" s="1">
         <v>41767.485532407409</v>
@@ -2029,13 +2029,13 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G9" s="1">
         <v>39877</v>
@@ -2044,16 +2044,16 @@
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M9" t="s">
         <v>49</v>
       </c>
       <c r="N9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O9">
         <v>2041008</v>
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="T9" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U9">
         <v>17459</v>
@@ -2080,19 +2080,19 @@
         <v>1</v>
       </c>
       <c r="W9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="X9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Y9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z9" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="AA9" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="AB9">
         <v>0</v>
@@ -2104,10 +2104,10 @@
         <v>3936</v>
       </c>
       <c r="AE9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="AF9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG9" s="1">
         <v>41789.629108796296</v>
@@ -2122,16 +2122,16 @@
         <v>1</v>
       </c>
       <c r="AK9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="AL9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AM9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AO9" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="AP9" s="1">
         <v>41845.622511574074</v>
@@ -2148,19 +2148,19 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G10" s="1">
         <v>39281</v>
       </c>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I10" t="s">
         <v>46</v>
@@ -2169,16 +2169,16 @@
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M10" t="s">
         <v>49</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O10">
         <v>2050280</v>
@@ -2196,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="T10" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U10">
         <v>15209</v>
@@ -2205,19 +2205,19 @@
         <v>1</v>
       </c>
       <c r="W10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="X10" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Y10" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z10" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="AA10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -2229,10 +2229,10 @@
         <v>659</v>
       </c>
       <c r="AE10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AF10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG10" s="1">
         <v>41580.016458333332</v>
@@ -2247,19 +2247,19 @@
         <v>3</v>
       </c>
       <c r="AK10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="AL10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="AM10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AN10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="AO10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="AP10" s="1">
         <v>41767.486342592594</v>
@@ -2277,13 +2277,13 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G11" s="1">
         <v>39877</v>
@@ -2292,16 +2292,16 @@
         <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M11" t="s">
         <v>49</v>
       </c>
       <c r="N11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O11">
         <v>2041008</v>
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="T11" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U11">
         <v>17039</v>
@@ -2328,19 +2328,19 @@
         <v>1</v>
       </c>
       <c r="W11" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="X11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="Y11" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="Z11" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="AA11" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -2352,10 +2352,10 @@
         <v>25</v>
       </c>
       <c r="AE11" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="AF11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG11" s="1">
         <v>41772.633888888886</v>
@@ -2370,16 +2370,16 @@
         <v>2</v>
       </c>
       <c r="AK11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="AL11" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="AM11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AO11" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="AP11" s="1">
         <v>41845.622499999998</v>

</xml_diff>